<commit_message>
doc: updated reference for new added data
</commit_message>
<xml_diff>
--- a/data_pocus/pocus-sources_name.xlsx
+++ b/data_pocus/pocus-sources_name.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10308"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\disdierm\Desktop\GitHub\covid19_pocus_ultrasound\data_pocus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jab/codevscovid/covid_detector/covid_detector/data_pocus/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E17115E-9433-C24B-8D82-2F6157FD61ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="convex" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="85">
   <si>
     <t>Cov-Atlas+(44).gif</t>
   </si>
@@ -258,12 +259,30 @@
   </si>
   <si>
     <t>Image too shallow to be really helpfull even if we can see some B-lines. Do not use in my opinion</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=HqPXJ0A0HCU</t>
+  </si>
+  <si>
+    <t>Reg-Youtube_Video_29_Lung_POCUS_left.mp4</t>
+  </si>
+  <si>
+    <t>Reg-Youtube_Video_29_Lung_POCUS_right.mp4</t>
+  </si>
+  <si>
+    <t>Reg-Youtube-Video_902_Lung_POCUS-left.mp4</t>
+  </si>
+  <si>
+    <t>Reg-Youtube-Video_902_Lung_POCUS.mp4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=pPQFvDI-kEg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1082,25 +1101,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="102.7109375" customWidth="1"/>
+    <col min="4" max="4" width="38.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="102.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -1117,7 +1136,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -1134,7 +1153,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -1151,7 +1170,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -1168,7 +1187,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -1185,7 +1204,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -1202,7 +1221,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -1219,7 +1238,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -1236,7 +1255,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -1253,7 +1272,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -1270,7 +1289,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -1287,7 +1306,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -1304,7 +1323,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -1321,7 +1340,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -1338,7 +1357,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -1355,7 +1374,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -1372,7 +1391,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -1389,7 +1408,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -1406,7 +1425,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -1423,7 +1442,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -1440,7 +1459,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>56</v>
       </c>
@@ -1457,7 +1476,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -1474,7 +1493,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>56</v>
       </c>
@@ -1491,7 +1510,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -1508,7 +1527,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -1525,7 +1544,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>56</v>
       </c>
@@ -1542,7 +1561,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>56</v>
       </c>
@@ -1559,7 +1578,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -1576,7 +1595,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -1593,7 +1612,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -1610,7 +1629,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>56</v>
       </c>
@@ -1627,7 +1646,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>56</v>
       </c>
@@ -1644,7 +1663,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>56</v>
       </c>
@@ -1661,7 +1680,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>56</v>
       </c>
@@ -1678,7 +1697,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>56</v>
       </c>
@@ -1695,7 +1714,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>56</v>
       </c>
@@ -1712,7 +1731,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>56</v>
       </c>
@@ -1729,7 +1748,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="2" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" s="2" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>57</v>
       </c>
@@ -1746,7 +1765,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>57</v>
       </c>
@@ -1763,7 +1782,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>57</v>
       </c>
@@ -1780,7 +1799,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>57</v>
       </c>
@@ -1797,68 +1816,116 @@
         <v>50</v>
       </c>
     </row>
+    <row r="43" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" t="s">
+        <v>80</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D44" t="s">
+        <v>81</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D45" t="s">
+        <v>82</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D46" t="s">
+        <v>83</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E8" r:id="rId1"/>
-    <hyperlink ref="E15" r:id="rId2"/>
-    <hyperlink ref="E23" r:id="rId3"/>
-    <hyperlink ref="E12" r:id="rId4"/>
-    <hyperlink ref="E31" r:id="rId5"/>
-    <hyperlink ref="E37" r:id="rId6"/>
-    <hyperlink ref="E36" r:id="rId7"/>
-    <hyperlink ref="E35" r:id="rId8"/>
-    <hyperlink ref="E34" r:id="rId9"/>
-    <hyperlink ref="E33" r:id="rId10"/>
-    <hyperlink ref="E9" r:id="rId11"/>
-    <hyperlink ref="E10" r:id="rId12"/>
-    <hyperlink ref="E11" r:id="rId13"/>
-    <hyperlink ref="E16" r:id="rId14"/>
-    <hyperlink ref="E17" r:id="rId15"/>
-    <hyperlink ref="E18" r:id="rId16"/>
-    <hyperlink ref="E19" r:id="rId17"/>
-    <hyperlink ref="E2" r:id="rId18"/>
-    <hyperlink ref="E3" r:id="rId19"/>
-    <hyperlink ref="E4" r:id="rId20"/>
-    <hyperlink ref="E5" r:id="rId21"/>
-    <hyperlink ref="E13" r:id="rId22"/>
-    <hyperlink ref="E14" r:id="rId23"/>
-    <hyperlink ref="E21" r:id="rId24"/>
-    <hyperlink ref="E22" r:id="rId25"/>
-    <hyperlink ref="E27" r:id="rId26"/>
-    <hyperlink ref="E28" r:id="rId27"/>
-    <hyperlink ref="E29" r:id="rId28"/>
-    <hyperlink ref="E32" r:id="rId29"/>
-    <hyperlink ref="E30" r:id="rId30" location="lungfindings" display="https://www.butterflynetwork.com/covid-19 - lungfindings"/>
-    <hyperlink ref="E24" r:id="rId31" location="lungfindings" display="https://www.butterflynetwork.com/covid-19 - lungfindings"/>
-    <hyperlink ref="E6" r:id="rId32" location="lungfindings" display="https://www.butterflynetwork.com/covid-19 - lungfindings"/>
-    <hyperlink ref="E7" r:id="rId33" location="lungfindings" display="https://www.butterflynetwork.com/covid-19 - lungfindings"/>
-    <hyperlink ref="E39" r:id="rId34"/>
-    <hyperlink ref="E40:E42" r:id="rId35" display="https://www.researchgate.net/publication/340286142_Proposal_for_international_standardization_of_the_use_of_lung_ultrasound_for_COVID-19_patients_a_simple_quantitative_reproducible_method"/>
+    <hyperlink ref="E8" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E15" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E23" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E12" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E31" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E37" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E36" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E35" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E34" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E33" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E9" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E10" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E11" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="E16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="E17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E18" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E19" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="E2" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="E3" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="E4" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="E5" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="E13" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="E14" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="E21" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="E22" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="E27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="E28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="E29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="E32" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="E30" r:id="rId30" location="lungfindings" display="https://www.butterflynetwork.com/covid-19 - lungfindings" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="E24" r:id="rId31" location="lungfindings" display="https://www.butterflynetwork.com/covid-19 - lungfindings" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="E6" r:id="rId32" location="lungfindings" display="https://www.butterflynetwork.com/covid-19 - lungfindings" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="E7" r:id="rId33" location="lungfindings" display="https://www.butterflynetwork.com/covid-19 - lungfindings" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="E39" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="E40:E42" r:id="rId35" display="https://www.researchgate.net/publication/340286142_Proposal_for_international_standardization_of_the_use_of_lung_ultrasound_for_COVID-19_patients_a_simple_quantitative_reproducible_method" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="E43" r:id="rId36" xr:uid="{BA1F1521-1019-1B41-ACD2-DC50EF241562}"/>
+    <hyperlink ref="E44" r:id="rId37" xr:uid="{4FD3E079-22AA-FE4F-AD7C-12246F79B070}"/>
+    <hyperlink ref="E45" r:id="rId38" xr:uid="{455D3E4A-CB4D-F14A-B5BC-188F0DA759BC}"/>
+    <hyperlink ref="E46" r:id="rId39" xr:uid="{FF4ED13B-E525-BD45-8DB7-C9A5E95E4606}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="28.5703125" customWidth="1"/>
-    <col min="4" max="4" width="121.28515625" customWidth="1"/>
+    <col min="3" max="3" width="28.5" customWidth="1"/>
+    <col min="4" max="4" width="121.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -1872,7 +1939,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -1886,7 +1953,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>57</v>
       </c>
@@ -1900,7 +1967,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>57</v>
       </c>
@@ -1914,7 +1981,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -1930,29 +1997,29 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3:D6" r:id="rId2" display="https://www.researchgate.net/publication/340286142_Proposal_for_international_standardization_of_the_use_of_lung_ultrasound_for_COVID-19_patients_a_simple_quantitative_reproducible_method"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D3:D6" r:id="rId2" display="https://www.researchgate.net/publication/340286142_Proposal_for_international_standardization_of_the_use_of_lung_ultrasound_for_COVID-19_patients_a_simple_quantitative_reproducible_method" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="44" customWidth="1"/>
-    <col min="4" max="4" width="142.7109375" customWidth="1"/>
+    <col min="4" max="4" width="142.6640625" customWidth="1"/>
     <col min="5" max="5" width="63" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
         <v>55</v>
       </c>
@@ -1960,7 +2027,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>57</v>
       </c>
@@ -1977,7 +2044,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>57</v>
       </c>
@@ -1994,7 +2061,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -2008,7 +2075,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -2022,7 +2089,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -2036,7 +2103,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -2050,7 +2117,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>57</v>
       </c>
@@ -2067,7 +2134,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -2086,10 +2153,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D8" r:id="rId3"/>
-    <hyperlink ref="D9" r:id="rId4"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="D8" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="D9" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: model train script
</commit_message>
<xml_diff>
--- a/data_pocus/pocus-sources_name.xlsx
+++ b/data_pocus/pocus-sources_name.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jab/codevscovid/covid_detector/covid_detector/data_pocus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E17115E-9433-C24B-8D82-2F6157FD61ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC7EE73-8AD9-D646-BFBA-A111FAE099E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1105,7 +1105,7 @@
   <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>